<commit_message>
FIX: structure ligand annotations
</commit_message>
<xml_diff>
--- a/structure_data/annotation/GPCRdb_structure_info.xlsx
+++ b/structure_data/annotation/GPCRdb_structure_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/protwis_vagrant/shared/data/protwis/gpcr/structure_data/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5068EBD-D9A7-2D44-BFDD-F426B93443AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93FA6DE-2634-744E-9F06-DE6E996353EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="500" windowWidth="32660" windowHeight="20540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10066" uniqueCount="1699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10065" uniqueCount="1701">
   <si>
     <t>PDB</t>
   </si>
@@ -5168,6 +5168,12 @@
   </si>
   <si>
     <t>DARPin D12</t>
+  </si>
+  <si>
+    <t>gtoplig:756</t>
+  </si>
+  <si>
+    <t>gtoplig:1815</t>
   </si>
 </sst>
 </file>
@@ -5637,8 +5643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="A637" workbookViewId="0">
-      <selection activeCell="A662" sqref="A662:XFD662"/>
+    <sheetView showFormulas="1" topLeftCell="A662" workbookViewId="0">
+      <selection activeCell="D684" sqref="D684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23847,8 +23853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
-      <selection activeCell="D209" sqref="D209:F209"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23860,7 +23866,7 @@
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="111.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="3.85546875" customWidth="1"/>
     <col min="10" max="10" width="6.28515625" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" customWidth="1"/>
@@ -34553,8 +34559,8 @@
       <c r="C438" s="4" t="s">
         <v>870</v>
       </c>
-      <c r="D438" s="5" t="s">
-        <v>849</v>
+      <c r="D438" s="5">
+        <v>457933</v>
       </c>
       <c r="E438" s="5" t="s">
         <v>846</v>
@@ -39519,7 +39525,7 @@
         <v>870</v>
       </c>
       <c r="D640" s="5" t="s">
-        <v>849</v>
+        <v>1699</v>
       </c>
       <c r="E640" s="5" t="s">
         <v>846</v>
@@ -39590,11 +39596,14 @@
       <c r="A643" s="4" t="s">
         <v>729</v>
       </c>
+      <c r="B643" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C643" s="4" t="s">
         <v>870</v>
       </c>
       <c r="D643" s="5" t="s">
-        <v>849</v>
+        <v>1699</v>
       </c>
       <c r="E643" s="5" t="s">
         <v>846</v>
@@ -39873,7 +39882,7 @@
         <v>870</v>
       </c>
       <c r="D654" s="5" t="s">
-        <v>849</v>
+        <v>1700</v>
       </c>
       <c r="E654" s="5" t="s">
         <v>846</v>
@@ -41486,14 +41495,14 @@
       <c r="C717" s="15" t="s">
         <v>870</v>
       </c>
-      <c r="D717" s="5" t="s">
-        <v>849</v>
+      <c r="D717" s="5">
+        <v>36511</v>
       </c>
       <c r="E717" s="7" t="s">
         <v>846</v>
       </c>
       <c r="F717" s="16" t="s">
-        <v>1556</v>
+        <v>1543</v>
       </c>
       <c r="G717" s="7" t="s">
         <v>872</v>

</xml_diff>

<commit_message>
FIX: updated structure annotation
</commit_message>
<xml_diff>
--- a/structure_data/annotation/GPCRdb_structure_info.xlsx
+++ b/structure_data/annotation/GPCRdb_structure_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vdc825/protwis_vagrant/shared/data/protwis/gpcr/structure_data/annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E936F4-2CE3-BE4D-9D81-EEC02BDAAD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91959F5-9A3D-6C4C-9BEB-66A4256D502E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="29700" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23908,8 +23908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="C740" sqref="C740"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>